<commit_message>
Random Customer With Random Order, StageScene Add DataManager
</commit_message>
<xml_diff>
--- a/Assets/Scripts/Data/Excels/CustomerTypeData.xlsx
+++ b/Assets/Scripts/Data/Excels/CustomerTypeData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="48">
   <si>
     <t>ID</t>
   </si>
@@ -20,6 +20,9 @@
   </si>
   <si>
     <t>BodyBaseType</t>
+  </si>
+  <si>
+    <t>Index</t>
   </si>
   <si>
     <t>Described</t>
@@ -413,22 +416,26 @@
     <col customWidth="1" min="1" max="1" width="8.71"/>
     <col customWidth="1" min="2" max="2" width="9.43"/>
     <col customWidth="1" min="3" max="3" width="13.43"/>
-    <col customWidth="1" min="4" max="4" width="10.71"/>
-    <col customWidth="1" min="5" max="6" width="8.71"/>
+    <col customWidth="1" min="4" max="4" width="5.86"/>
+    <col customWidth="1" min="5" max="5" width="10.71"/>
+    <col customWidth="1" min="6" max="7" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" ht="16.5" customHeight="1">
@@ -436,13 +443,16 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" ht="16.5" customHeight="1">
@@ -450,13 +460,16 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" ht="16.5" customHeight="1">
@@ -464,13 +477,16 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" ht="16.5" customHeight="1">
@@ -478,13 +494,16 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" ht="16.5" customHeight="1">
@@ -492,13 +511,16 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" ht="16.5" customHeight="1">
@@ -506,13 +528,16 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="D7" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" ht="16.5" customHeight="1">
@@ -520,13 +545,16 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>14</v>
+        <v>6</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" ht="16.5" customHeight="1">
@@ -534,13 +562,16 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>15</v>
+        <v>6</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" ht="16.5" customHeight="1">
@@ -548,13 +579,16 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
+      </c>
+      <c r="D10" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="11" ht="16.5" customHeight="1">
@@ -562,13 +596,16 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" ht="16.5" customHeight="1">
@@ -576,13 +613,16 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="13" ht="16.5" customHeight="1">
@@ -590,13 +630,16 @@
         <v>12.0</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="D13" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14" ht="16.5" customHeight="1">
@@ -604,13 +647,16 @@
         <v>13.0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="15" ht="16.5" customHeight="1">
@@ -618,13 +664,16 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
+      </c>
+      <c r="D15" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="16" ht="16.5" customHeight="1">
@@ -632,13 +681,16 @@
         <v>15.0</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
+      </c>
+      <c r="D16" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="17" ht="16.5" customHeight="1">
@@ -646,13 +698,16 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="18" ht="16.5" customHeight="1">
@@ -660,13 +715,16 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
+      </c>
+      <c r="D18" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="19" ht="16.5" customHeight="1">
@@ -674,13 +732,16 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
+      </c>
+      <c r="D19" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="20" ht="16.5" customHeight="1">
@@ -688,13 +749,16 @@
         <v>19.0</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="21" ht="16.5" customHeight="1">
@@ -702,13 +766,16 @@
         <v>20.0</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="D21" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="22" ht="16.5" customHeight="1">
@@ -716,13 +783,16 @@
         <v>21.0</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
+      </c>
+      <c r="D22" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="23" ht="16.5" customHeight="1">
@@ -730,13 +800,16 @@
         <v>22.0</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="24" ht="16.5" customHeight="1">
@@ -744,13 +817,16 @@
         <v>23.0</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+      <c r="D24" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="25" ht="16.5" customHeight="1">
@@ -758,13 +834,16 @@
         <v>24.0</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
+      </c>
+      <c r="D25" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="26" ht="16.5" customHeight="1">
@@ -772,13 +851,16 @@
         <v>25.0</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="27" ht="16.5" customHeight="1">
@@ -786,13 +868,16 @@
         <v>26.0</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
+      </c>
+      <c r="D27" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="28" ht="16.5" customHeight="1">
@@ -800,13 +885,16 @@
         <v>27.0</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>36</v>
+        <v>28</v>
+      </c>
+      <c r="D28" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="29" ht="16.5" customHeight="1">
@@ -814,13 +902,16 @@
         <v>28.0</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D29" s="1" t="s">
         <v>38</v>
+      </c>
+      <c r="D29" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="30" ht="16.5" customHeight="1">
@@ -828,13 +919,16 @@
         <v>29.0</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="D30" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="31" ht="16.5" customHeight="1">
@@ -842,13 +936,16 @@
         <v>30.0</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
+      </c>
+      <c r="D31" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="32" ht="16.5" customHeight="1">
@@ -856,13 +953,16 @@
         <v>31.0</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
+      </c>
+      <c r="D32" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="33" ht="16.5" customHeight="1">
@@ -870,13 +970,16 @@
         <v>32.0</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="D33" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="34" ht="16.5" customHeight="1">
@@ -884,13 +987,16 @@
         <v>33.0</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
+      </c>
+      <c r="D34" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="35" ht="16.5" customHeight="1">
@@ -898,13 +1004,16 @@
         <v>34.0</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
+      </c>
+      <c r="D35" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="36" ht="16.5" customHeight="1">
@@ -912,13 +1021,16 @@
         <v>35.0</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
+      </c>
+      <c r="D36" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="37" ht="16.5" customHeight="1">
@@ -926,13 +1038,16 @@
         <v>36.0</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
+      </c>
+      <c r="D37" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="38" ht="16.5" customHeight="1"/>

</xml_diff>